<commit_message>
Added old ECO Changes
Inserted old ECO changes from previous BOMs
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v1-130906.xlsx
+++ b/Bill of Materials/core-bom-v1-130906.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="217">
   <si>
     <t>Device</t>
   </si>
@@ -804,6 +804,27 @@
   </si>
   <si>
     <t>130906</t>
+  </si>
+  <si>
+    <t>core-bom-v025-090213</t>
+  </si>
+  <si>
+    <t>Updated buffer P/N from NL17SZ125 to NL17SZ125XV5T2G to specify SOT-553 package</t>
+  </si>
+  <si>
+    <t>9/4</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Updated antenna designator from A1 to ANT1</t>
+  </si>
+  <si>
+    <t>Added the MFG P/N of C8,C9 is CL10C100DBANNNC, MFG name is RongFu</t>
+  </si>
+  <si>
+    <t>Charlie</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1397,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1489,13 +1510,13 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="329" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="329" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="329"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="329" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,9 +1529,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="329" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="339">
     <cellStyle name="Bad" xfId="124" builtinId="27"/>
@@ -2182,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2207,10 +2225,10 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="2:10" ht="16" thickBot="1">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="57"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="21">
         <v>41523</v>
       </c>
@@ -2261,14 +2279,14 @@
       <c r="C6" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10">
@@ -2394,10 +2412,10 @@
       <c r="G11" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="55" t="s">
         <v>204</v>
       </c>
       <c r="J11" s="5" t="s">
@@ -2513,7 +2531,7 @@
       <c r="C16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="54" t="s">
         <v>198</v>
       </c>
       <c r="E16" s="5"/>
@@ -2523,10 +2541,10 @@
       <c r="G16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="59" t="s">
+      <c r="H16" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="I16" s="61" t="s">
+      <c r="I16" s="56" t="s">
         <v>200</v>
       </c>
       <c r="J16" s="5" t="s">
@@ -3248,28 +3266,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M111"/>
+  <dimension ref="A2:M112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="53" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="54" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73" style="54" customWidth="1"/>
-    <col min="6" max="7" width="14.33203125" style="54" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="54" customWidth="1"/>
-    <col min="9" max="9" width="16" style="53" customWidth="1"/>
-    <col min="10" max="10" width="15" style="53" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="53" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="52" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="53" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73" style="53" customWidth="1"/>
+    <col min="6" max="7" width="14.33203125" style="53" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="53" customWidth="1"/>
+    <col min="9" max="9" width="16" style="52" customWidth="1"/>
+    <col min="10" max="10" width="15" style="52" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="52" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="39" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" style="42" customWidth="1"/>
-    <col min="14" max="14" width="13.5" style="53" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="53"/>
+    <col min="14" max="14" width="13.5" style="52" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="52"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" s="39" customFormat="1">
@@ -3357,48 +3375,48 @@
       <c r="L9" s="38"/>
     </row>
     <row r="10" spans="2:13" s="44" customFormat="1" ht="21" customHeight="1">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58" t="s">
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
       <c r="L10" s="45"/>
     </row>
     <row r="11" spans="2:13" s="44" customFormat="1" ht="15">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="60"/>
+      <c r="E11" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="60" t="s">
         <v>187</v>
       </c>
       <c r="L11" s="45"/>
     </row>
     <row r="12" spans="2:13" s="44" customFormat="1" ht="15">
-      <c r="B12" s="58"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="43" t="s">
         <v>188</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
       <c r="L12" s="45"/>
     </row>
     <row r="13" spans="2:13" s="48" customFormat="1" ht="15">
@@ -3406,19 +3424,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="46" t="s">
-        <v>197</v>
-      </c>
       <c r="E13" s="47" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="F13" s="46" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="G13" s="46" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="2:13" s="48" customFormat="1" ht="15">
@@ -3426,19 +3444,19 @@
         <v>2</v>
       </c>
       <c r="C14" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="46" t="s">
-        <v>197</v>
-      </c>
       <c r="E14" s="47" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="F14" s="46" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="2:13" s="48" customFormat="1" ht="15">
@@ -3446,19 +3464,19 @@
         <v>3</v>
       </c>
       <c r="C15" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="D15" s="46" t="s">
-        <v>197</v>
-      </c>
       <c r="E15" s="47" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="2:13" s="48" customFormat="1" ht="15">
@@ -3472,7 +3490,7 @@
         <v>197</v>
       </c>
       <c r="E16" s="47" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F16" s="46" t="s">
         <v>195</v>
@@ -3485,31 +3503,61 @@
       <c r="B17" s="46">
         <v>5</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="C17" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="18" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B18" s="46">
         <v>6</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
+      <c r="C18" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="19" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B19" s="46">
         <v>7</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
+      <c r="C19" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="20" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B20" s="46">
@@ -3611,35 +3659,35 @@
       <c r="F29" s="46"/>
       <c r="G29" s="46"/>
     </row>
-    <row r="30" spans="2:7" s="51" customFormat="1" ht="15">
+    <row r="30" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B30" s="46">
         <v>18</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-    </row>
-    <row r="31" spans="2:7" s="51" customFormat="1" ht="15">
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+    </row>
+    <row r="31" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B31" s="46">
         <v>19</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-    </row>
-    <row r="32" spans="2:7" s="51" customFormat="1" ht="15">
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+    </row>
+    <row r="32" spans="2:7" s="48" customFormat="1" ht="15">
       <c r="B32" s="46">
         <v>20</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
     </row>
     <row r="33" spans="2:7" s="51" customFormat="1" ht="15">
       <c r="B33" s="46">
@@ -3921,7 +3969,7 @@
       <c r="F60" s="49"/>
       <c r="G60" s="49"/>
     </row>
-    <row r="61" spans="1:13" s="52" customFormat="1" ht="15">
+    <row r="61" spans="1:13" s="51" customFormat="1" ht="15">
       <c r="B61" s="46">
         <v>49</v>
       </c>
@@ -3931,46 +3979,56 @@
       <c r="F61" s="49"/>
       <c r="G61" s="49"/>
     </row>
-    <row r="62" spans="1:13" s="39" customFormat="1">
-      <c r="A62" s="53"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="54"/>
-      <c r="M62" s="42"/>
+    <row r="62" spans="1:13" s="51" customFormat="1" ht="15">
+      <c r="B62" s="46">
+        <v>50</v>
+      </c>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
     </row>
     <row r="63" spans="1:13" s="39" customFormat="1">
-      <c r="A63" s="53"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
+      <c r="A63" s="52"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
       <c r="I63" s="53"/>
       <c r="J63" s="53"/>
       <c r="K63" s="53"/>
       <c r="M63" s="42"/>
     </row>
-    <row r="111" spans="1:13" s="54" customFormat="1">
-      <c r="A111" s="53"/>
-      <c r="B111" s="42" t="s">
+    <row r="64" spans="1:13" s="39" customFormat="1">
+      <c r="A64" s="52"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="53"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="52"/>
+      <c r="M64" s="42"/>
+    </row>
+    <row r="112" spans="1:13" s="53" customFormat="1">
+      <c r="A112" s="52"/>
+      <c r="B112" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="C111" s="42"/>
-      <c r="D111" s="42"/>
-      <c r="I111" s="53"/>
-      <c r="J111" s="53"/>
-      <c r="K111" s="53"/>
-      <c r="L111" s="39"/>
-      <c r="M111" s="42"/>
+      <c r="C112" s="42"/>
+      <c r="D112" s="42"/>
+      <c r="I112" s="52"/>
+      <c r="J112" s="52"/>
+      <c r="K112" s="52"/>
+      <c r="L112" s="39"/>
+      <c r="M112" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>